<commit_message>
Feat: Excel Data Json Convert
- 엑셀 데이터 Json 변환 하도록 수정
</commit_message>
<xml_diff>
--- a/logSheet.xlsx
+++ b/logSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/programmer/Desktop/Git/game-data-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DBBA5E-466A-CD49-A77E-6DBA06E2B29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C9EFE9-8C6B-4444-88A4-FCDA9CFC32D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="2440" windowWidth="25820" windowHeight="15100" xr2:uid="{9A59ABBB-740E-4CA1-BCEB-12671D992041}"/>
+    <workbookView xWindow="12580" yWindow="500" windowWidth="21020" windowHeight="20500" activeTab="1" xr2:uid="{9A59ABBB-740E-4CA1-BCEB-12671D992041}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Actor 아이디 값</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -152,6 +152,22 @@
   </si>
   <si>
     <t>Consume</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEMTEMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_id2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_id3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -214,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -237,13 +253,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -263,6 +290,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -581,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F931D9-CE19-43AB-B9DF-A4D9742E2F82}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -744,10 +786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8A1E3B-A7AE-DB40-BAE9-73E7CEE05557}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -758,7 +800,7 @@
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="46" customHeight="1">
+    <row r="1" spans="1:9" ht="46" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -780,8 +822,14 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -803,8 +851,14 @@
       <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -815,7 +869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -835,8 +889,14 @@
       <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -856,8 +916,14 @@
       <c r="G5" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="6">
         <v>10</v>
       </c>
@@ -877,8 +943,14 @@
       <c r="G6" s="6">
         <v>10004323</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="11">
+        <v>1000230</v>
+      </c>
+      <c r="I6" s="11">
+        <v>123123123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="6">
         <v>11</v>
       </c>
@@ -897,6 +969,12 @@
       </c>
       <c r="G7" s="6">
         <v>10000234</v>
+      </c>
+      <c r="H7" s="11">
+        <v>24324234</v>
+      </c>
+      <c r="I7" s="11">
+        <v>123123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chore: Log Shett Table 이름 변경
</commit_message>
<xml_diff>
--- a/logSheet.xlsx
+++ b/logSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/programmer/Desktop/Git/game-data-tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\programmer\Desktop\git\pl\game-data-tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C9EFE9-8C6B-4444-88A4-FCDA9CFC32D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3740A3EB-4698-4D1E-9ED8-55AE460A3C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12580" yWindow="500" windowWidth="21020" windowHeight="20500" activeTab="1" xr2:uid="{9A59ABBB-740E-4CA1-BCEB-12671D992041}"/>
+    <workbookView xWindow="-45" yWindow="-14145" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{9A59ABBB-740E-4CA1-BCEB-12671D992041}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>Actor 아이디 값</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,6 +168,10 @@
   </si>
   <si>
     <t>skill_id3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -175,7 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -624,20 +628,20 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="5" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="46.5" customHeight="1">
+    <row r="1" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,7 +664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -683,7 +687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -694,7 +698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -704,7 +708,9 @@
       <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
@@ -715,7 +721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -725,7 +731,9 @@
       <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
@@ -736,7 +744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>10</v>
       </c>
@@ -757,7 +765,7 @@
         <v>10004323</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>11</v>
       </c>
@@ -789,18 +797,18 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="46" customHeight="1">
+    <row r="1" spans="1:9" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -829,7 +837,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -858,7 +866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -869,61 +877,65 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>10</v>
       </c>
@@ -950,7 +962,7 @@
         <v>123123123</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>11</v>
       </c>

</xml_diff>